<commit_message>
Commit by Farheen: Work on bugs and Item master
</commit_message>
<xml_diff>
--- a/InVanWebApp/ExcelFileFormat/Download-Format-Item.xlsx
+++ b/InVanWebApp/ExcelFileFormat/Download-Format-Item.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC7F319-DC8F-446F-B9BB-5DA65C43ED95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCDE8BC-B5FA-4EB7-98AA-23F8E3E810C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Item_Name</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>TM_0001</t>
+  </si>
+  <si>
+    <t>UnitPrice</t>
   </si>
 </sst>
 </file>
@@ -102,46 +105,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -448,11 +422,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,13 +435,14 @@
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="39.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="39.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,16 +456,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -503,18 +481,21 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="F2">
+      <c r="E2" s="2">
+        <v>40.049999999999997</v>
+      </c>
+      <c r="G2">
         <v>10000</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  <conditionalFormatting sqref="D2:E1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1048576">
+  <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -524,7 +505,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select the valid category of Item!" sqref="C2:C1048576" xr:uid="{84BA0521-BADB-4A9B-8BDE-B14DB9FD51A9}">
       <formula1>"Finished Good, Semi-Finished Good, Raw Material"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Stock can't be negative or in string!" sqref="F2:F1048576" xr:uid="{30325471-035A-4D0E-82E3-306D60C397A0}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Stock can't be negative or in string!" sqref="G2:G1048576" xr:uid="{30325471-035A-4D0E-82E3-306D60C397A0}">
       <formula1>-1</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Commit by Farheen: Bug fixing.
</commit_message>
<xml_diff>
--- a/InVanWebApp/ExcelFileFormat/Download-Format-Item.xlsx
+++ b/InVanWebApp/ExcelFileFormat/Download-Format-Item.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCDE8BC-B5FA-4EB7-98AA-23F8E3E810C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829AD8E2-F731-4324-A5A5-5CD3C75398FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,7 +115,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -426,7 +456,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,13 +520,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:E1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="D2:D1048576">
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select the valid type of Item!" sqref="B2:B1048576" xr:uid="{986ACAFF-8C39-4250-BEE8-587A4699D184}">
@@ -510,5 +540,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>